<commit_message>
Added error checking and refactored to allow optional risk-free rate (set to 0 or single number).
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE7C60C-4D52-4685-955A-03EC0A6BBA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F6603C-7A54-44B0-B823-3204B3A5749C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="2700" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="5580" yWindow="3540" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>RFR</t>
   </si>
@@ -130,19 +130,26 @@
   </si>
   <si>
     <t>Tracking Error</t>
+  </si>
+  <si>
+    <t>Bear Market</t>
+  </si>
+  <si>
+    <t>Bull Market</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.00000%"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;?????_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -187,7 +194,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -210,6 +217,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,9 +551,12 @@
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -554,8 +566,14 @@
       <c r="K1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -577,8 +595,26 @@
       <c r="L2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -602,8 +638,32 @@
       <c r="L3" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P3" cm="1">
+        <f t="array" ref="P3:P10">_xlfn._xlws.FILTER(B3:B17,$C$3:$C$17&lt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" cm="1">
+        <f t="array" ref="Q3:Q10">_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0)</f>
+        <v>-9.4000423002005284E-5</v>
+      </c>
+      <c r="R3" cm="1">
+        <f t="array" ref="R3:R10">_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" cm="1">
+        <f t="array" ref="T3:T9">_xlfn._xlws.FILTER(B3:B17,$C$3:$C$17&gt;0)</f>
+        <v>8.2200000000032247E-5</v>
+      </c>
+      <c r="U3" cm="1">
+        <f t="array" ref="U3:U9">_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0)</f>
+        <v>3.2231746255595439E-4</v>
+      </c>
+      <c r="V3" cm="1">
+        <f t="array" ref="V3:V9">_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0)</f>
+        <v>3.1331199999999892E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>8.2200000000032247E-5</v>
       </c>
@@ -627,8 +687,26 @@
       <c r="L4" s="14">
         <v>3.1331199999999892E-3</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>8.2199729546594824E-5</v>
+      </c>
+      <c r="Q4">
+        <v>-7.2435597111886185E-4</v>
+      </c>
+      <c r="R4">
+        <v>-1.2263622560784171E-3</v>
+      </c>
+      <c r="T4">
+        <v>8.2193243715389386E-5</v>
+      </c>
+      <c r="U4">
+        <v>7.2296678179091245E-3</v>
+      </c>
+      <c r="V4">
+        <v>1.113068622437674E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>8.2193243715389386E-5</v>
       </c>
@@ -652,8 +730,26 @@
       <c r="L5" s="14">
         <v>1.113068622437674E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>2.4657891991952674E-4</v>
+      </c>
+      <c r="Q5">
+        <v>-3.1356092824675885E-3</v>
+      </c>
+      <c r="R5">
+        <v>-6.0585660461631718E-5</v>
+      </c>
+      <c r="T5">
+        <v>8.2186488541191594E-5</v>
+      </c>
+      <c r="U5">
+        <v>2.8791074766820746E-3</v>
+      </c>
+      <c r="V5">
+        <v>-1.5737770653512229E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>8.2186488541191594E-5</v>
       </c>
@@ -677,8 +773,26 @@
       <c r="L6" s="14">
         <v>-1.5737770653512229E-3</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>8.2192419748716716E-5</v>
+      </c>
+      <c r="Q6">
+        <v>-4.895586322955392E-3</v>
+      </c>
+      <c r="R6">
+        <v>-1.1019876585149913E-2</v>
+      </c>
+      <c r="T6">
+        <v>8.219269974518717E-5</v>
+      </c>
+      <c r="U6">
+        <v>2.5817555938039138E-3</v>
+      </c>
+      <c r="V6">
+        <v>2.1230588697924713E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8.2199729546594824E-5</v>
       </c>
@@ -702,8 +816,26 @@
       <c r="L7" s="14">
         <v>-1.2263622560784171E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>2.4657697605667828E-4</v>
+      </c>
+      <c r="Q7">
+        <v>-9.6922866109405703E-5</v>
+      </c>
+      <c r="R7">
+        <v>2.7731910686723538E-4</v>
+      </c>
+      <c r="T7">
+        <v>8.2185944660473353E-5</v>
+      </c>
+      <c r="U7">
+        <v>3.4268223708289192E-4</v>
+      </c>
+      <c r="V7">
+        <v>-1.2212168590912675E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2.4657891991952674E-4</v>
       </c>
@@ -727,8 +859,26 @@
       <c r="L8" s="14">
         <v>-6.0585660461631718E-5</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>8.2185381613975039E-5</v>
+      </c>
+      <c r="Q8">
+        <v>-8.4163942535884217E-3</v>
+      </c>
+      <c r="R8">
+        <v>-4.8789385894569826E-3</v>
+      </c>
+      <c r="T8">
+        <v>8.2199175897912369E-5</v>
+      </c>
+      <c r="U8">
+        <v>1.9955233758750524E-5</v>
+      </c>
+      <c r="V8">
+        <v>5.190551166665891E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>8.219269974518717E-5</v>
       </c>
@@ -752,8 +902,26 @@
       <c r="L9" s="14">
         <v>2.1230588697924713E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>8.2191847036172661E-5</v>
+      </c>
+      <c r="Q9">
+        <v>-2.4289165022262083E-3</v>
+      </c>
+      <c r="R9">
+        <v>-6.3539265847126769E-3</v>
+      </c>
+      <c r="T9">
+        <v>8.2198603090999356E-5</v>
+      </c>
+      <c r="U9">
+        <v>6.1585653610194413E-3</v>
+      </c>
+      <c r="V9">
+        <v>7.5949356979387872E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8.2185944660473353E-5</v>
       </c>
@@ -777,8 +945,17 @@
       <c r="L10" s="14">
         <v>-1.2212168590912675E-3</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>8.218509209156899E-5</v>
+      </c>
+      <c r="Q10">
+        <v>-5.3163264620735839E-3</v>
+      </c>
+      <c r="R10">
+        <v>2.6039764394154563E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>8.2199175897912369E-5</v>
       </c>
@@ -803,7 +980,7 @@
         <v>5.190551166665891E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8.2192419748716716E-5</v>
       </c>
@@ -827,8 +1004,16 @@
       <c r="L12" s="14">
         <v>-1.1019876585149913E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P12" s="17" cm="1">
+        <f t="array" ref="P12">SLOPE(_xlfn.ANCHORARRAY(R3)-_xlfn.ANCHORARRAY(P3),_xlfn.ANCHORARRAY(Q3)-_xlfn.ANCHORARRAY(P3))</f>
+        <v>0.53164017255257146</v>
+      </c>
+      <c r="T12" s="17" cm="1">
+        <f t="array" ref="T12">SLOPE(_xlfn.ANCHORARRAY(V3)-_xlfn.ANCHORARRAY(T3),_xlfn.ANCHORARRAY(U3)-_xlfn.ANCHORARRAY(T3))</f>
+        <v>1.0869193898495133</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2.4657697605667828E-4</v>
       </c>
@@ -853,7 +1038,7 @@
         <v>2.7731910686723538E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>8.2185381613975039E-5</v>
       </c>
@@ -878,7 +1063,7 @@
         <v>-4.8789385894569826E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>8.2198603090999356E-5</v>
       </c>
@@ -903,7 +1088,7 @@
         <v>7.5949356979387872E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>8.2191847036172661E-5</v>
       </c>
@@ -1003,17 +1188,17 @@
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="8">
-        <f>_xlfn.COVARIANCE.P(C3:C17,$C$3:$C$17)/_xlfn.VAR.P($C$3:$C$17)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="D21" s="8">
-        <f>_xlfn.COVARIANCE.P(D3:D17,$C$3:$C$17)/_xlfn.VAR.P($C$3:$C$17)</f>
-        <v>0.9424115940712039</v>
+      <c r="C21" s="8" cm="1">
+        <f t="array" ref="C21">_xlfn.COVARIANCE.P(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.P($C$3:$C$17-$B$3:$B$17)</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="8" cm="1">
+        <f t="array" ref="D21">_xlfn.COVARIANCE.P(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.P($C$3:$C$17-$B$3:$B$17)</f>
+        <v>0.94109509071871278</v>
       </c>
       <c r="G21" s="9" cm="1">
-        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17)</f>
-        <v>0.94241159407120412</v>
+        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17,B3:B17)</f>
+        <v>0.94109509071871278</v>
       </c>
       <c r="H21" s="10">
         <f>D21-G21</f>
@@ -1029,16 +1214,16 @@
         <v>13</v>
       </c>
       <c r="C22" s="8" cm="1">
-        <f t="array" ref="C22">SLOPE(_xlfn._xlws.FILTER(C3:C17,C3:C17&gt;0),_xlfn._xlws.FILTER(C3:C17,C3:C17&gt;0))</f>
+        <f t="array" ref="C22">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
         <v>1</v>
       </c>
       <c r="D22" s="8" cm="1">
-        <f t="array" ref="D22">SLOPE(_xlfn._xlws.FILTER(D3:D17,C3:C17&gt;0),_xlfn._xlws.FILTER(C3:C17,C3:C17&gt;0))</f>
-        <v>1.0869212641710992</v>
+        <f t="array" ref="D22">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
+        <v>1.0869193898495133</v>
       </c>
       <c r="G22" s="9" cm="1">
-        <f t="array" ref="G22">_xll.BullBeta(D3:D17,C3:C17)</f>
-        <v>1.0869212641710995</v>
+        <f t="array" ref="G22">_xll.BullBeta(D3:D17,C3:C17,B3:B17)</f>
+        <v>1.0869193898495135</v>
       </c>
       <c r="H22" s="10">
         <f t="shared" ref="H22:H30" si="1">D22-G22</f>
@@ -1054,23 +1239,23 @@
         <v>14</v>
       </c>
       <c r="C23" s="8" cm="1">
-        <f t="array" ref="C23">SLOPE(_xlfn._xlws.FILTER(C3:C17,C3:C17&lt;0),_xlfn._xlws.FILTER(C3:C17,C3:C17&lt;0))</f>
+        <f t="array" ref="C23">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
         <v>1</v>
       </c>
       <c r="D23" s="8" cm="1">
-        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,C3:C17&lt;0),_xlfn._xlws.FILTER(C3:C17,C3:C17&lt;0))</f>
-        <v>0.54207326774062659</v>
+        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
+        <v>0.53164017255257146</v>
       </c>
       <c r="G23" s="9" cm="1">
-        <f t="array" ref="G23">_xll.BearBeta(D3:D17,C3:C17)</f>
-        <v>0.54207326774062647</v>
+        <f t="array" ref="G23">_xll.BearBeta(D3:D17,C3:C17,B3:B17)</f>
+        <v>0.53164017255257146</v>
       </c>
       <c r="H23" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L23" t="e" cm="1">
-        <f t="array" ref="L23">_xll.BearBeta(L3:L17,K3:K17)</f>
+        <f t="array" ref="L23">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1084,11 +1269,11 @@
       </c>
       <c r="D24" s="8">
         <f>D22/D23</f>
-        <v>2.0051187336748981</v>
+        <v>2.0444643688810649</v>
       </c>
       <c r="G24" s="9" cm="1">
-        <f t="array" ref="G24">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
-        <v>2.005118733674899</v>
+        <f t="array" ref="G24">_xll.BetaTimingRatio(D3:D17,C3:C17,B3:B17)</f>
+        <v>2.0444643688810649</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="1"/>
@@ -1129,15 +1314,15 @@
       <c r="B26" s="1"/>
       <c r="C26" s="8">
         <f>(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/C21</f>
-        <v>-4.7023516149291577E-4</v>
+        <v>-4.7023516149291567E-4</v>
       </c>
       <c r="D26" s="8">
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
-        <v>2.9990416146271969E-4</v>
+        <v>3.0032369912462605E-4</v>
       </c>
       <c r="G26" s="9" cm="1">
-        <f t="array" ref="G26">_xll.TreynorIndex(D3:D17,B3:B17,G21)</f>
-        <v>2.9990416146271964E-4</v>
+        <f t="array" ref="G26">_xll.TreynorIndex(D3:D17,D21,B3:B17)</f>
+        <v>3.0032369912462605E-4</v>
       </c>
       <c r="H26" s="10">
         <f t="shared" si="1"/>
@@ -1179,11 +1364,11 @@
       </c>
       <c r="G28" s="13" cm="1">
         <f t="array" ref="G28">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2578822700353814E-4</v>
+        <v>7.2516916083697341E-4</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="1"/>
-        <v>-6.1906616656472874E-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,12 +1413,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
+      <c r="G33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Fama's Deomposition of the excess return and Revised Sharpe Ratio.
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F6603C-7A54-44B0-B823-3204B3A5749C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4803BA-7865-4FD6-9C3E-F9D94C32616F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3540" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$28</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$29</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>RFR</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Bull Market</t>
+  </si>
+  <si>
+    <t>Revised Sharpe Ratio</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -219,6 +222,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -535,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
@@ -1226,7 +1232,7 @@
         <v>1.0869193898495135</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" ref="H22:H30" si="1">D22-G22</f>
+        <f t="shared" ref="H22:H31" si="1">D22-G22</f>
         <v>0</v>
       </c>
       <c r="L22" cm="1">
@@ -1309,62 +1315,64 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="8" cm="1">
+        <f t="array" ref="C26">(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(C3:C17-$B$3:$B$17)</f>
+        <v>-0.11273902975687349</v>
+      </c>
+      <c r="D26" s="8" cm="1">
+        <f t="array" ref="D26">(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(D3:D17-$B$3:$B$17)</f>
+        <v>5.1676557020390534E-2</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="G26" s="9" cm="1">
+        <f t="array" ref="G26">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
+        <v>5.1676557020390521E-2</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="8">
+      <c r="B27" s="1"/>
+      <c r="C27" s="8">
         <f>(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/C21</f>
         <v>-4.7023516149291567E-4</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D27" s="8">
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
         <v>3.0032369912462605E-4</v>
       </c>
-      <c r="G26" s="9" cm="1">
-        <f t="array" ref="G26">_xll.TreynorIndex(D3:D17,D21,B3:B17)</f>
+      <c r="G27" s="9" cm="1">
+        <f t="array" ref="G27">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
         <v>3.0032369912462605E-4</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H27" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C28" s="8">
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(C3:C17))*(C19-$B$19)+$B$19</f>
         <v>-3.7160406004862107E-4</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="8">
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(D3:D17))*(D19-$B$19)+$B$19</f>
         <v>3.138111214532042E-4</v>
       </c>
-      <c r="G27" s="9" cm="1">
-        <f t="array" ref="G27">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
+      <c r="G28" s="9" cm="1">
+        <f t="array" ref="G28">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
         <v>3.1381112145320415E-4</v>
-      </c>
-      <c r="H27" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="12" cm="1">
-        <f t="array" ref="C28">INTERCEPT(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="12" cm="1">
-        <f t="array" ref="D28">INTERCEPT(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>7.2516916083697341E-4</v>
-      </c>
-      <c r="G28" s="13" cm="1">
-        <f t="array" ref="G28">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2516916083697341E-4</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="1"/>
@@ -1373,16 +1381,19 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="C29" s="12" cm="1">
+        <f t="array" ref="C29">INTERCEPT(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
+        <v>0</v>
+      </c>
       <c r="D29" s="12" cm="1">
-        <f t="array" ref="D29">_xlfn.STDEV.S(D3:D17-C3:C17)</f>
-        <v>3.816440754566235E-3</v>
+        <f t="array" ref="D29">INTERCEPT(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
+        <v>7.2516916083697341E-4</v>
       </c>
       <c r="G29" s="13" cm="1">
-        <f t="array" ref="G29">_xll.TrackingError(D3:D17,C3:C17)</f>
-        <v>3.816440754566235E-3</v>
+        <f t="array" ref="G29">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
+        <v>7.2516916083697341E-4</v>
       </c>
       <c r="H29" s="10">
         <f t="shared" si="1"/>
@@ -1391,15 +1402,19 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="8" cm="1">
-        <f t="array" ref="D30">(AVERAGE(D3:D17)-AVERAGE(C3:C17))/_xlfn.STDEV.S(D3:D17-C3:C17)</f>
-        <v>0.19726975178765843</v>
-      </c>
-      <c r="G30" s="8" cm="1">
-        <f t="array" ref="G30">_xll.InformationRatio(D3:D17,C3:C17)</f>
-        <v>0.19726975178765843</v>
+        <v>21</v>
+      </c>
+      <c r="C30" s="12" cm="1">
+        <f t="array" ref="C30">_xlfn.STDEV.S(C3:C17-$C$3:$C$17)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="12" cm="1">
+        <f t="array" ref="D30">_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
+        <v>3.816440754566235E-3</v>
+      </c>
+      <c r="G30" s="13" cm="1">
+        <f t="array" ref="G30">_xll.TrackingError(D3:D17,C3:C17)</f>
+        <v>3.816440754566235E-3</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="1"/>
@@ -1407,19 +1422,93 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="G31" s="10"/>
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8" cm="1">
+        <f t="array" ref="D31">(AVERAGE(D3:D17)-AVERAGE($C$3:$C$17))/_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
+        <v>0.19726975178765843</v>
+      </c>
+      <c r="G31" s="8" cm="1">
+        <f t="array" ref="G31">_xll.InformationRatio(D3:D17,C3:C17)</f>
+        <v>0.19726975178765843</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="G33" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="G34" s="18" t="str" cm="1">
+        <f t="array" ref="G34:H40">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+        <v>Risk Premium</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2.8263315887266938E-4</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <v>Due to Risk</v>
+      </c>
+      <c r="H35" s="1">
+        <v>-4.4253600196430404E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <v>Due to Selectivity</v>
+      </c>
+      <c r="H36" s="1">
+        <v>7.2516916083697341E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <v>Due to Investor's Risk</v>
+      </c>
+      <c r="H37" s="1">
+        <v>-6.1130570994079043E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <v>Due to Manager's Risk</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1.6876970797648637E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <v>Diversification</v>
+      </c>
+      <c r="H39" s="1">
+        <v>8.4527012988867047E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <v>Net Selectivity</v>
+      </c>
+      <c r="H40" s="1">
+        <v>6.4064214784810634E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>